<commit_message>
Moved BOM xlsx to proper folder.
</commit_message>
<xml_diff>
--- a/PCB/CentralBoard/LightController_BOM.xlsx
+++ b/PCB/CentralBoard/LightController_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Lonnie II\Desktop\School\Controls\snc-closedloop\PCB\CentralBoard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nomad\Documents\Rowan\Junior\Spring\Systems &amp; Control\Final Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFE6DB36-FEBF-4B14-BAEC-0E6BBDD6A6C5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{777FE162-DAE0-406A-875A-9479276325EA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="14280"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8952" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LightController_BOM" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
     <t>Supplier and ref</t>
   </si>
   <si>
-    <t>B+1 B-1</t>
+    <t>B+1;B-1</t>
   </si>
   <si>
     <t>MountingHole_2.2mm_M2_Pad</t>
@@ -49,7 +49,7 @@
     <t>Mounting_Hole_PAD</t>
   </si>
   <si>
-    <t>P1 P3 P5 P6 P7 P8 P9 P10 P11 P12 P13 P14 P15 P16 P17 P18</t>
+    <t>P1;P3;P5;P6;P7;P8;P9;P10;P11;P12;P13;P14;P15;P16;P17;P18</t>
   </si>
   <si>
     <t>Pin_Header_Straight_1x03_Pitch2.54mm</t>
@@ -58,7 +58,7 @@
     <t>CONN_01X03</t>
   </si>
   <si>
-    <t>P2 P4</t>
+    <t>P2;P4</t>
   </si>
   <si>
     <t>Pin_Header_Straight_1x10_Pitch2.54mm</t>
@@ -103,7 +103,7 @@
     <t>PCA9685</t>
   </si>
   <si>
-    <t>U4 U5 U6 U7</t>
+    <t>U4;U5;U6;U7</t>
   </si>
   <si>
     <t>MSOP-8_3x3mm_Pitch0.65mm</t>
@@ -112,7 +112,7 @@
     <t>BA4510FVM-GTR</t>
   </si>
   <si>
-    <t>C1 C7 C9 C12 C14 C16 C18</t>
+    <t>C1;C7;C9;C12;C14;C16;C18</t>
   </si>
   <si>
     <t>C_0603</t>
@@ -121,13 +121,13 @@
     <t>100n</t>
   </si>
   <si>
-    <t>C2 C8</t>
+    <t>C2;C8</t>
   </si>
   <si>
     <t>10n</t>
   </si>
   <si>
-    <t>C3 C5 C6 C10 C11 C13 C15 C17</t>
+    <t>C3;C5;C6;C10;C11;C13;C15;C17</t>
   </si>
   <si>
     <t>10u</t>
@@ -139,7 +139,7 @@
     <t>1u</t>
   </si>
   <si>
-    <t>R1 R2 R5 R6 R7 R8 R9 R10 R14 R15 R19 R20 R24 R25</t>
+    <t>R1;R2;R5;R6;R7;R8;R9;R10;R14;R15;R19;R20;R24;R25</t>
   </si>
   <si>
     <t>R_0603</t>
@@ -154,28 +154,28 @@
     <t>R4</t>
   </si>
   <si>
-    <t>R11 R16 R21 R26</t>
-  </si>
-  <si>
-    <t>100k</t>
-  </si>
-  <si>
-    <t>R12 R13 R17 R18 R22 R23 R27 R28</t>
+    <t>R11;R16;R21;R26</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>R12;R17;R22;R27</t>
   </si>
   <si>
     <t>2.4k</t>
   </si>
   <si>
-    <t>R29 R30 R31 R32</t>
-  </si>
-  <si>
-    <t>1.2k</t>
+    <t>R13;R18;R23;R28</t>
+  </si>
+  <si>
+    <t>5.1k</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -653,8 +653,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1009,21 +1015,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" customWidth="1"/>
-    <col min="5" max="5" width="40.85546875" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="53.83984375" customWidth="1"/>
+    <col min="3" max="3" width="33.68359375" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="20.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1032,7 +1040,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -1042,8 +1050,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -1052,15 +1060,15 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -1069,15 +1077,15 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1086,15 +1094,15 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -1103,15 +1111,15 @@
       <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -1120,15 +1128,15 @@
       <c r="C6" t="s">
         <v>19</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -1137,15 +1145,15 @@
       <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>1</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -1154,15 +1162,15 @@
       <c r="C8" t="s">
         <v>25</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>1</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -1171,15 +1179,15 @@
       <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>4</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -1188,15 +1196,15 @@
       <c r="C10" t="s">
         <v>31</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>7</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" t="s">
@@ -1205,15 +1213,15 @@
       <c r="C11" t="s">
         <v>31</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>2</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" t="s">
@@ -1222,15 +1230,15 @@
       <c r="C12" t="s">
         <v>31</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>8</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" t="s">
@@ -1239,15 +1247,15 @@
       <c r="C13" t="s">
         <v>31</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>1</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" t="s">
@@ -1256,15 +1264,15 @@
       <c r="C14" t="s">
         <v>40</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>14</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" t="s">
@@ -1273,15 +1281,15 @@
       <c r="C15" t="s">
         <v>40</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>1</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <v>240</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" t="s">
@@ -1290,15 +1298,15 @@
       <c r="C16" t="s">
         <v>40</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <v>1</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <v>750</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" t="s">
@@ -1307,15 +1315,15 @@
       <c r="C17" t="s">
         <v>40</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
         <v>4</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" t="s">
@@ -1324,15 +1332,15 @@
       <c r="C18" t="s">
         <v>40</v>
       </c>
-      <c r="D18">
-        <v>8</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D18" s="2">
+        <v>4</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" t="s">
@@ -1341,10 +1349,10 @@
       <c r="C19" t="s">
         <v>40</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>4</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="1" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>